<commit_message>
update import excel nhan vien detail
</commit_message>
<xml_diff>
--- a/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/Employee_Detail_Template.xlsx
+++ b/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/Employee_Detail_Template.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\Source\NET CORE\ASP.NET CORE\HRMNS\HRMS\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hop Dong" sheetId="1" r:id="rId1"/>
     <sheet name="Qua trinh cong tac" sheetId="2" r:id="rId2"/>
     <sheet name="Tinh Trạng Ho So" sheetId="3" r:id="rId3"/>
+    <sheet name="LoaiDH_CONST" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Mã Hợp Đồng</t>
   </si>
@@ -80,6 +81,39 @@
   </si>
   <si>
     <t>Ảnh Thẻ</t>
+  </si>
+  <si>
+    <t>H2105001</t>
+  </si>
+  <si>
+    <t>HD20210501</t>
+  </si>
+  <si>
+    <t>hd lao dong</t>
+  </si>
+  <si>
+    <t>Hợp Đồng 1 năm lần 2</t>
+  </si>
+  <si>
+    <t>Hợp Đồng Thử Việc</t>
+  </si>
+  <si>
+    <t>Hợp Đồng 1 năm lần 1</t>
+  </si>
+  <si>
+    <t>Hợp Đồng Không Thời Hạn</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -95,7 +129,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +139,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,10 +182,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +473,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +497,7 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -461,16 +511,42 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3">
+        <v>44317</v>
+      </c>
+      <c r="F2" s="3">
+        <v>44317</v>
+      </c>
+      <c r="G2" s="3">
+        <v>44682</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>LoaiDH_CONST!$A$1:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -524,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,5 +647,79 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>LoaiDH_CONST!$E$1:$E$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:H2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1">
+        <v>14</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>